<commit_message>
Add to weintek var export file new variables
</commit_message>
<xml_diff>
--- a/Var.xlsx
+++ b/Var.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="20115" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="210" windowWidth="20115" windowHeight="7935" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Structs" sheetId="1" r:id="rId1"/>
@@ -979,7 +979,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>